<commit_message>
Deleted commented code, tested all scenarios in different situations, autopilot controller now has circular checkbox
</commit_message>
<xml_diff>
--- a/lander/circular_orbit_altitudes.xlsx
+++ b/lander/circular_orbit_altitudes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnbrown/Documents/GitHub/lander/lander/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36BA3D70-B678-8243-8965-80E3EE01CE55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D239015E-120A-1145-9799-CF33A10C15D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38700" yWindow="2760" windowWidth="28180" windowHeight="16720" xr2:uid="{2AE6916A-B8CF-7E47-9BD9-74ACE6C53F28}"/>
   </bookViews>
@@ -131,16 +131,14 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -171,10 +169,43 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="#,##0.000000000" sourceLinked="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
+                      <a:t>y = 1.6883873497x - 2,587,894.3661202100</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
+                      <a:t>R² = 0.9970112435</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -206,56 +237,134 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$20</c:f>
+              <c:f>Sheet1!$A$1:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>3526000</c:v>
+                  <c:v>5500000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3506000</c:v>
+                  <c:v>6000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3496000</c:v>
+                  <c:v>6500000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3486000</c:v>
+                  <c:v>7000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3516000</c:v>
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3900000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6500000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3900000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5500000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6500000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7500000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3900000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$20</c:f>
+              <c:f>Sheet1!$B$1:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>3595000</c:v>
+                  <c:v>6537910</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3559000</c:v>
+                  <c:v>7395880</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3542000</c:v>
+                  <c:v>8286530</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3526000</c:v>
+                  <c:v>9182160</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3577000</c:v>
+                  <c:v>10107600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4037580</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6556470</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7420520</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8309000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9215470</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10133100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4062140</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6703850</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7565600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8455870</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9362670</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10279100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4178350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7A0F-6C4D-A5D6-9B0BDD60348E}"/>
+              <c16:uniqueId val="{00000000-0391-3940-A980-4CD9B8C1C407}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -267,11 +376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2052488335"/>
-        <c:axId val="2052518351"/>
+        <c:axId val="558516031"/>
+        <c:axId val="558732527"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2052488335"/>
+        <c:axId val="558516031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -328,12 +437,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2052518351"/>
+        <c:crossAx val="558732527"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2052518351"/>
+        <c:axId val="558732527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -390,7 +499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2052488335"/>
+        <c:crossAx val="558516031"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1006,23 +1115,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD5E9948-C659-804D-B706-94902AEAC33C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098B5310-55C4-4C48-9F39-71AB95EE403E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1340,52 +1449,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5899481A-6874-DE42-922A-3D1040EA96AF}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>3526000</v>
+        <v>5500000</v>
       </c>
       <c r="B1">
-        <v>3595000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6537910</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>3506000</v>
+        <v>6000000</v>
       </c>
       <c r="B2">
-        <v>3559000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7395880</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3496000</v>
+        <v>6500000</v>
       </c>
       <c r="B3">
-        <v>3542000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8286530</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3486000</v>
+        <v>7000000</v>
       </c>
       <c r="B4">
-        <v>3526000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9182160</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3516000</v>
+        <v>7500000</v>
       </c>
       <c r="B5">
-        <v>3577000</v>
+        <v>10107600</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3900000</v>
+      </c>
+      <c r="B6">
+        <v>4037580</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5500000</v>
+      </c>
+      <c r="B7">
+        <v>6556470</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6000000</v>
+      </c>
+      <c r="B8">
+        <v>7420520</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6500000</v>
+      </c>
+      <c r="B9">
+        <v>8309000</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7000000</v>
+      </c>
+      <c r="B10">
+        <v>9215470</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7500000</v>
+      </c>
+      <c r="B11">
+        <v>10133100</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3900000</v>
+      </c>
+      <c r="B12">
+        <v>4062140</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5500000</v>
+      </c>
+      <c r="B13">
+        <v>6703850</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6000000</v>
+      </c>
+      <c r="B14">
+        <v>7565600</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>6500000</v>
+      </c>
+      <c r="B15">
+        <v>8455870</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>7000000</v>
+      </c>
+      <c r="B16">
+        <v>9362670</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>7500000</v>
+      </c>
+      <c r="B17">
+        <v>10279100</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3900000</v>
+      </c>
+      <c r="B18">
+        <v>4178350</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>